<commit_message>
Gabriel Finalizando todos os erros
</commit_message>
<xml_diff>
--- a/planilha_robo_iss.xlsx
+++ b/planilha_robo_iss.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas-ti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas-ti\Documents\workSpace\roboIss\RoboIss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F43E78-7299-4EF3-BB8F-3B0AEABC244A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BEFAF2-6006-457F-A358-BFC79FD2A6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9FBABEF1-810A-4A33-A2A2-C20BD378460C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="5318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="5319">
   <si>
     <t>CNPJ</t>
   </si>
@@ -15991,7 +15991,10 @@
     <t>E</t>
   </si>
   <si>
-    <t>193815</t>
+    <t>198549</t>
+  </si>
+  <si>
+    <t>200053</t>
   </si>
 </sst>
 </file>
@@ -16395,7 +16398,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16447,10 +16450,10 @@
         <v>5317</v>
       </c>
       <c r="C2" s="4">
-        <v>45659</v>
+        <v>45673</v>
       </c>
       <c r="D2">
-        <v>6613400</v>
+        <v>6619305</v>
       </c>
       <c r="E2" t="s">
         <v>5316</v>
@@ -16462,7 +16465,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="6">
-        <v>4181.7</v>
+        <v>2083.96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -16470,10 +16473,10 @@
         <v>5314</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5317</v>
+        <v>5318</v>
       </c>
       <c r="C3" s="4">
-        <v>45659</v>
+        <v>45679</v>
       </c>
       <c r="D3">
         <v>6613400</v>
@@ -16488,7 +16491,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="6">
-        <v>4181.7</v>
+        <v>2637.28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gabriel correçao de erros robo
</commit_message>
<xml_diff>
--- a/planilha_robo_iss.xlsx
+++ b/planilha_robo_iss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas-ti\Documents\workSpace\roboIss\RoboIss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BEFAF2-6006-457F-A358-BFC79FD2A6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798A5321-300D-4926-8BBF-08A4CE541CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9FBABEF1-810A-4A33-A2A2-C20BD378460C}"/>
   </bookViews>
@@ -15982,19 +15982,19 @@
     <t>Nº DOCUMENTO</t>
   </si>
   <si>
-    <t>44.097.674/0001-21</t>
-  </si>
-  <si>
     <t>SERIE</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>198549</t>
-  </si>
-  <si>
-    <t>200053</t>
+    <t>00.604.122/0001-97</t>
+  </si>
+  <si>
+    <t>2369123</t>
+  </si>
+  <si>
+    <t>2374187</t>
   </si>
 </sst>
 </file>
@@ -16398,7 +16398,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16430,7 +16430,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5315</v>
+        <v>5314</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -16444,54 +16444,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5314</v>
+        <v>5316</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5317</v>
       </c>
       <c r="C2" s="4">
-        <v>45673</v>
+        <v>45659</v>
       </c>
       <c r="D2">
         <v>6619305</v>
       </c>
       <c r="E2" t="s">
-        <v>5316</v>
+        <v>5315</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
+        <v>2352</v>
       </c>
       <c r="H2" s="6">
-        <v>2083.96</v>
+        <v>9972.01</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5314</v>
+        <v>5316</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5318</v>
       </c>
       <c r="C3" s="4">
-        <v>45679</v>
+        <v>45672</v>
       </c>
       <c r="D3">
-        <v>6613400</v>
+        <v>6619305</v>
       </c>
       <c r="E3" t="s">
-        <v>5316</v>
+        <v>5315</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
+        <v>2352</v>
       </c>
       <c r="H3" s="6">
-        <v>2637.28</v>
+        <v>1445.75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gabriel solucionando possiveis erros!
</commit_message>
<xml_diff>
--- a/planilha_robo_iss.xlsx
+++ b/planilha_robo_iss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas-ti\Documents\workSpace\roboIss\RoboIss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5FA1CA-89BE-4777-8F87-45706D372231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A517BA79-F33D-491D-8736-38845C481D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5579" uniqueCount="5320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5579" uniqueCount="5321">
   <si>
     <t>AC</t>
   </si>
@@ -15972,9 +15972,6 @@
     <t>00.604.122/0001-97</t>
   </si>
   <si>
-    <t>2369123</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -15982,6 +15979,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>44.097.674/0001-21</t>
+  </si>
+  <si>
+    <t>00198549</t>
   </si>
 </sst>
 </file>
@@ -16102,7 +16105,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -16413,7 +16416,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16456,28 +16459,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5315</v>
+        <v>5319</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>5316</v>
+        <v>5320</v>
       </c>
       <c r="C2" s="11">
-        <v>45659</v>
+        <v>45673</v>
       </c>
       <c r="D2" s="18">
         <v>6619305</v>
       </c>
       <c r="E2" t="s">
-        <v>5317</v>
+        <v>5316</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>5269</v>
+        <v>4949</v>
       </c>
       <c r="H2" s="13">
-        <v>9972.01</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16485,7 +16488,7 @@
         <v>5315</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>5318</v>
+        <v>5317</v>
       </c>
       <c r="C3" s="11">
         <v>45672</v>
@@ -16494,7 +16497,7 @@
         <v>6619305</v>
       </c>
       <c r="E3" t="s">
-        <v>5317</v>
+        <v>5316</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -16508,7 +16511,7 @@
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>5319</v>
+        <v>5318</v>
       </c>
       <c r="C4" s="11"/>
       <c r="G4" s="12"/>

</xml_diff>

<commit_message>
Gabriel correçao de erros
</commit_message>
<xml_diff>
--- a/planilha_robo_iss.xlsx
+++ b/planilha_robo_iss.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geise Ferreira\OneDrive\Documentos\Robô Iss Fortaleza\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas-ti\Documents\workSpace\roboIss\RoboIss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847A4102-BED9-41C2-B62A-09A96914B500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222B032-B7DA-4ECE-B263-F65BA37B6E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9FBABEF1-810A-4A33-A2A2-C20BD378460C}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9FBABEF1-810A-4A33-A2A2-C20BD378460C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5588" uniqueCount="5323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="5318">
   <si>
     <t>CNPJ</t>
   </si>
@@ -15988,25 +15988,10 @@
     <t>E</t>
   </si>
   <si>
-    <t>36.462.778/0001-60</t>
-  </si>
-  <si>
-    <t>4166</t>
-  </si>
-  <si>
-    <t>16846</t>
-  </si>
-  <si>
-    <t>12.607.697/0001-42</t>
-  </si>
-  <si>
-    <t>6445</t>
-  </si>
-  <si>
-    <t>04.740.876/0001-25</t>
-  </si>
-  <si>
-    <t>383738</t>
+    <t>25.322.949/0002-10</t>
+  </si>
+  <si>
+    <t>16999</t>
   </si>
 </sst>
 </file>
@@ -16412,7 +16397,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16465,7 +16450,7 @@
         <v>5317</v>
       </c>
       <c r="C2" s="4">
-        <v>45659</v>
+        <v>45690</v>
       </c>
       <c r="D2">
         <v>6202300</v>
@@ -16474,13 +16459,13 @@
         <v>5315</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>3560</v>
+        <v>4473</v>
       </c>
       <c r="H2" s="6">
-        <v>181.17</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -16488,10 +16473,10 @@
         <v>5316</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5318</v>
+        <v>5317</v>
       </c>
       <c r="C3" s="4">
-        <v>45661</v>
+        <v>45690</v>
       </c>
       <c r="D3">
         <v>6202300</v>
@@ -16500,66 +16485,25 @@
         <v>5315</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>3560</v>
+        <v>4473</v>
       </c>
       <c r="H3" s="6">
-        <v>267.22000000000003</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5319</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5320</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45661</v>
-      </c>
-      <c r="D4">
-        <v>6202300</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5315</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>3088</v>
-      </c>
-      <c r="H4" s="6">
-        <v>70</v>
-      </c>
+      <c r="C4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5321</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5322</v>
-      </c>
-      <c r="C5" s="4">
-        <v>45658</v>
-      </c>
-      <c r="D5">
-        <v>7490104</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>5315</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>4575</v>
-      </c>
-      <c r="H5" s="6">
-        <v>6000</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>

</xml_diff>